<commit_message>
Auto stash before merge of "tomHome" and "origin/master"
</commit_message>
<xml_diff>
--- a/TimetrackingTom.xlsx
+++ b/TimetrackingTom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9C29B3-22EB-40B9-9F90-2894148F4E97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EEE559-B52D-4B5D-9D9A-589D9403697F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Git work + arduino play</t>
+  </si>
+  <si>
+    <t>1830- 2030</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +465,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -495,7 +509,7 @@
       </c>
       <c r="C9" s="1">
         <f>SUBTOTAL(109,C2:C8)</f>
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="D9" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated kingle bells and time sheet
</commit_message>
<xml_diff>
--- a/TimetrackingTom.xlsx
+++ b/TimetrackingTom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EEE559-B52D-4B5D-9D9A-589D9403697F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B095D4-E4DA-46DF-BA8D-366A152B2DFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t>1830- 2030</t>
+  </si>
+  <si>
+    <t>Sunday 22.4.18</t>
+  </si>
+  <si>
+    <t>Sunday 15.4.18</t>
+  </si>
+  <si>
+    <t>1000-1600</t>
+  </si>
+  <si>
+    <t>Getting the bastard to work</t>
+  </si>
+  <si>
+    <t>1000-1230</t>
+  </si>
+  <si>
+    <t>Trying to connect to device</t>
   </si>
 </sst>
 </file>
@@ -414,7 +432,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,16 +497,32 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -509,7 +543,7 @@
       </c>
       <c r="C9" s="1">
         <f>SUBTOTAL(109,C2:C8)</f>
-        <v>3.5</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1"/>
     </row>

</xml_diff>

<commit_message>
removed some redundant items and created some folders for organisation
</commit_message>
<xml_diff>
--- a/TimetrackingTom.xlsx
+++ b/TimetrackingTom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B095D4-E4DA-46DF-BA8D-366A152B2DFF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB3FCB4-CE7E-463A-9628-3F4E3838FB3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,10 +73,10 @@
     <t>Getting the bastard to work</t>
   </si>
   <si>
-    <t>1000-1230</t>
-  </si>
-  <si>
     <t>Trying to connect to device</t>
+  </si>
+  <si>
+    <t>1000-1300</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,13 +515,13 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
       </c>
       <c r="C9" s="1">
         <f>SUBTOTAL(109,C2:C8)</f>
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="D9" s="1"/>
     </row>

</xml_diff>